<commit_message>
📈 Actualizo análisis de sentimientos y resultados en Excel
</commit_message>
<xml_diff>
--- a/Trabajo_final/resultados_text_analytics.xlsx
+++ b/Trabajo_final/resultados_text_analytics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>review30.txt</t>
+          <t>review68.txt</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,25 +478,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>tres semanas, error interno, solicitud, alternativa</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>tres semanas (DateTime), solicitud (Skill)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>comunicación, Buena transparencia, email, paso, proceso</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles), Bueña (https://en.wikipedia.org/wiki/Bueña)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>review29.txt</t>
+          <t>review33.txt</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,24 +511,24 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>préstamo, trato, personal, Sentí, dudas</t>
+          <t>documentación, 15 días, desembolso, tiempo, urgencia</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>personal (PersonType)</t>
+          <t>15 días (DateTime), urgencia (Event)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+          <t>United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>review16.txt</t>
+          <t>review58.txt</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -538,29 +538,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>préstamo, una semana, observaciones, documentos, asesores, pacientes</t>
+          <t>Cero seguimiento, préstamo, banco</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>una semana (DateTime), asesores (PersonType), pacientes (PersonType)</t>
+          <t>banco (Location)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+          <t>Computer Entertainment Rating Organization (https://en.wikipedia.org/wiki/Computer_Entertainment_Rating_Organization), Yo (film) (https://en.wikipedia.org/wiki/Yo_(film)), Tienen (https://en.wikipedia.org/wiki/Tienen)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>review1.txt</t>
+          <t>review80.txt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -575,24 +575,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Caja Municipal ADV, dos días, préstamo, dinero, cuenta, proceso, personal</t>
+          <t>pequeño error, Excelente gestión, documento, asesor</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Caja Municipal ADV (Organization), dos días (DateTime), personal (PersonType)</t>
+          <t>asesor (PersonType), gestión (Skill)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Spondias mombin (https://en.wikipedia.org/wiki/Spondias_mombin), C.S.D. Municipal (https://en.wikipedia.org/wiki/C.S.D._Municipal)</t>
+          <t>HUBO (https://en.wikipedia.org/wiki/HUBO), Dobla (https://en.wikipedia.org/wiki/Dobla)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>review6.txt</t>
+          <t>review30.txt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -602,29 +602,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>cinco días, tres pasos simples, préstamo, evaluación, solicitud, firma, personal</t>
+          <t>tres semanas, error interno, solicitud, alternativa</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>cinco días (DateTime), solicitud (Skill), evaluación (Skill), personal (PersonType)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>El (deity) (https://en.wikipedia.org/wiki/El_(deity))</t>
-        </is>
-      </c>
+          <t>tres semanas (DateTime), solicitud (Skill)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>review25.txt</t>
+          <t>review29.txt</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -639,24 +635,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>trámite, evaluación, 11 días, firma, desembolso, dinero</t>
+          <t>préstamo, trato, personal, Sentí, dudas</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>evaluación (Skill), firma (Skill), 11 días (DateTime)</t>
+          <t>personal (PersonType)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Aura (Ozuna album) (https://en.wikipedia.org/wiki/Aura_(Ozuna_album))</t>
+          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>review24.txt</t>
+          <t>review16.txt</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -666,29 +662,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>mixed</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>coordinación, información, personal, falta, áreas</t>
+          <t>préstamo, una semana, observaciones, documentos, asesores, pacientes</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>personal (PersonType), coordinación (Skill)</t>
+          <t>una semana (DateTime), asesores (PersonType), pacientes (PersonType)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Él (film) (https://en.wikipedia.org/wiki/Él_(film))</t>
+          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>review23.txt</t>
+          <t>review1.txt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -698,29 +694,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15 días, préstamo, experiencia, terrible, motivos, tiempo, dinero</t>
+          <t>Caja Municipal ADV, dos días, préstamo, dinero, cuenta, proceso, personal</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>15 días (DateTime)</t>
+          <t>Caja Municipal ADV (Organization), dos días (DateTime), personal (PersonType)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Uña (https://en.wikipedia.org/wiki/Uña), Espère (https://en.wikipedia.org/wiki/Espère)</t>
+          <t>Spondias mombin (https://en.wikipedia.org/wiki/Spondias_mombin), C.S.D. Municipal (https://en.wikipedia.org/wiki/C.S.D._Municipal)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>review19.txt</t>
+          <t>review6.txt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -730,29 +726,29 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>atención, trámite, dos semanas, tiempos, dinero</t>
+          <t>cinco días, tres pasos simples, préstamo, evaluación, solicitud, firma, personal</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>dos semanas (DateTime)</t>
+          <t>cinco días (DateTime), solicitud (Skill), evaluación (Skill), personal (PersonType)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
+          <t>El (deity) (https://en.wikipedia.org/wiki/El_(deity))</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>review17.txt</t>
+          <t>review39.txt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -762,29 +758,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Excelente atención, préstamo, 48 horas, transparencia, personal</t>
+          <t>primera cuota, error administrativo, mucha molestia, llamadas, cobro, grave</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>48 horas (DateTime), personal (PersonType)</t>
+          <t>primera (Quantity), error administrativo (Event)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>English language (https://en.wikipedia.org/wiki/English_language), Dobla (https://en.wikipedia.org/wiki/Dobla)</t>
+          <t>United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>review22.txt</t>
+          <t>review70.txt</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -794,25 +790,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>agencia ADV, proceso, documentos</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>agencia ADV (Location)</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>otros lados, trámite, tasa, pena</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>La Mé (https://en.wikipedia.org/wiki/La_Mé), Súper (https://en.wikipedia.org/wiki/Súper), Valió la Pena (https://en.wikipedia.org/wiki/Valió_la_Pena)</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>review7.txt</t>
+          <t>review66.txt</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -822,29 +818,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>mixed</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>préstamo personal, Caja ADV, atención, dinero, menos, 24 horas, asesora</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Caja ADV (Organization), 24 horas (DateTime), atención (Skill), asesora (PersonType)</t>
-        </is>
-      </c>
+          <t>tantos, documentos, listado, requisitos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
+          <t>.gr (https://en.wikipedia.org/wiki/.gr)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>review10.txt</t>
+          <t>review25.txt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -854,29 +846,29 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>atención, desembolso, tasas, plazos</t>
+          <t>trámite, evaluación, 11 días, firma, desembolso, dinero</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>atención (Skill), cuatro días (DateTime)</t>
+          <t>evaluación (Skill), firma (Skill), 11 días (DateTime)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
+          <t>Aura (Ozuna album) (https://en.wikipedia.org/wiki/Aura_(Ozuna_album))</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>review18.txt</t>
+          <t>review24.txt</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -886,25 +878,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>tres días, Buen trato, proceso, formularios</t>
+          <t>coordinación, información, personal, falta, áreas</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>tres días (DateTime)</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>personal (PersonType), coordinación (Skill)</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Él (film) (https://en.wikipedia.org/wiki/Él_(film))</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>review26.txt</t>
+          <t>review23.txt</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -914,29 +910,29 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>préstamo, varios documentos, atención, proceso, tasas</t>
+          <t>15 días, préstamo, experiencia, terrible, motivos, tiempo, dinero</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>proceso (Skill), atención (Skill)</t>
+          <t>15 días (DateTime)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo), Latin (https://en.wikipedia.org/wiki/Latin)</t>
+          <t>Uña (https://en.wikipedia.org/wiki/Uña), Espère (https://en.wikipedia.org/wiki/Espère)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>review14.txt</t>
+          <t>review19.txt</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -946,29 +942,29 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Excelente servicio, Caja ADV, día, un, dinero</t>
+          <t>atención, trámite, dos semanas, tiempos, dinero</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>un día (DateTime)</t>
+          <t>dos semanas (DateTime)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Dobla (https://en.wikipedia.org/wiki/Dobla), English language (https://en.wikipedia.org/wiki/English_language)</t>
+          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>review2.txt</t>
+          <t>review17.txt</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -978,29 +974,29 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>verificación, documentos, desembolso, personal</t>
+          <t>Excelente atención, préstamo, 48 horas, transparencia, personal</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>personal (PersonType), verificación (Skill)</t>
+          <t>48 horas (DateTime), personal (PersonType)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ASEAN University Network (https://en.wikipedia.org/wiki/ASEAN_University_Network)</t>
+          <t>English language (https://en.wikipedia.org/wiki/English_language), Dobla (https://en.wikipedia.org/wiki/Dobla)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>review13.txt</t>
+          <t>review61.txt</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1015,24 +1011,24 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>cinco días exactos, préstamo, varios pasos, asesora</t>
+          <t>otros bancos, buena oferta, tasa</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>cinco días (DateTime), asesora (PersonType), profesional (Skill)</t>
+          <t>bancos (Location)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo), Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
+          <t>Uña (https://en.wikipedia.org/wiki/Uña)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>review8.txt</t>
+          <t>review22.txt</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1042,17 +1038,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>varios documentos, trámite, proceso, media, personal</t>
+          <t>agencia ADV, proceso, documentos</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>una semana y media (DateTime), personal (PersonType)</t>
+          <t>agencia ADV (Location)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -1060,7 +1056,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>review5.txt</t>
+          <t>review7.txt</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1075,24 +1071,24 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>tres días, Caja ADV, experiencia, solicitud, desembolso</t>
+          <t>préstamo personal, Caja ADV, atención, dinero, menos, 24 horas, asesora</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>tres días (DateTime), ADV (Skill)</t>
+          <t>Caja ADV (Organization), 24 horas (DateTime), atención (Skill), asesora (PersonType)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Mii (https://en.wikipedia.org/wiki/Mii)</t>
+          <t>Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>review15.txt</t>
+          <t>review36.txt</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1102,17 +1098,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>buena tasa de, Buen servicio, interés, WhatsApp, dudas</t>
+          <t>flujo digital, sistema, documentos, proceso</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>cuatro días (DateTime), WhatsApp (Organization)</t>
+          <t>flujo digital (Skill)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
@@ -1120,7 +1116,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>review21.txt</t>
+          <t>review10.txt</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1130,25 +1126,29 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>mixed</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>tres días, préstamo, dos semanas, Nadie, respuesta, clara</t>
+          <t>atención, desembolso, tasas, plazos</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>dos semanas (DateTime)</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
+          <t>atención (Skill), cuatro días (DateTime)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>review12.txt</t>
+          <t>review67.txt</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1158,25 +1158,21 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>diez días, evaluación, atención, comunicación, desembolso, avance</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>diez días (DateTime), comunicación (Skill)</t>
-        </is>
-      </c>
+          <t>tasa, facilidad, rapidez, proceso</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>review28.txt</t>
+          <t>review18.txt</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1186,29 +1182,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>pésima experiencia, Caja ADV, documentos, errores, nada</t>
+          <t>tres días, Buen trato, proceso, formularios</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>documentos (Product), Caja ADV (Organization)</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Spondias mombin (https://en.wikipedia.org/wiki/Spondias_mombin)</t>
-        </is>
-      </c>
+          <t>tres días (DateTime)</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>review27.txt</t>
+          <t>review26.txt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1218,29 +1210,29 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>mixed</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>mucha gente, una hora, agencia, sistema</t>
+          <t>préstamo, varios documentos, atención, proceso, tasas</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>agencia (Location), una hora (DateTime), ágil (Skill)</t>
+          <t>proceso (Skill), atención (Skill)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>English language (https://en.wikipedia.org/wiki/English_language)</t>
+          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo), Latin (https://en.wikipedia.org/wiki/Latin)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>review20.txt</t>
+          <t>review78.txt</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1250,29 +1242,25 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>dos días, préstamo, estudios, asesor, momento, cliente</t>
+          <t>proceso, tasa, pena</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>dos días (DateTime), asesor (PersonType), cliente (PersonType)</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
-        </is>
-      </c>
+          <t>(4 días (DateTime)</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>review3.txt</t>
+          <t>review72.txt</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1282,29 +1270,29 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Excelente servicio, préstamo, trámite, negocio, 48 horas, paso</t>
+          <t>atención personalizada, desembolso, ejecutiva</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>servicio (Skill), 48 horas (DateTime)</t>
+          <t>5 días (DateTime), ejecutiva (PersonType)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Dobla (https://en.wikipedia.org/wiki/Dobla), Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
+          <t>Él (film) (https://en.wikipedia.org/wiki/Él_(film))</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>review11.txt</t>
+          <t>review14.txt</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1319,24 +1307,24 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>tres días, Caja ADV, préstamo, buena experiencia, agencia, respeto, rapidez</t>
+          <t>Excelente servicio, Caja ADV, día, un, dinero</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>agencia (Location), Caja ADV (Organization), tres días (DateTime)</t>
+          <t>un día (DateTime)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>English language (https://en.wikipedia.org/wiki/English_language), Isidoro Caja de la Jara (https://en.wikipedia.org/wiki/Isidoro_Caja_de_la_Jara), El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+          <t>Dobla (https://en.wikipedia.org/wiki/Dobla), English language (https://en.wikipedia.org/wiki/English_language)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>review4.txt</t>
+          <t>review73.txt</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1346,52 +1334,1548 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>nueve días, préstamo, proceso, trato, tiempos</t>
+          <t>sitio web, archivos, grandes, estabilidad</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>nueve días (DateTime)</t>
+          <t>sitio (Skill)</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+          <t>El Sitio (https://en.wikipedia.org/wiki/El_Sitio)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>review2.txt</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>verificación, documentos, desembolso, personal</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>personal (PersonType), verificación (Skill)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ASEAN University Network (https://en.wikipedia.org/wiki/ASEAN_University_Network)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>review55.txt</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>intereses, capital, pena, necesidad</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>review75.txt</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Un punto medio, garante, seguro, desgravamen</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>review13.txt</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>cinco días exactos, préstamo, varios pasos, asesora</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>cinco días (DateTime), asesora (PersonType), profesional (Skill)</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo), Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>review32.txt</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>interés, campaña, tasa</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>campaña (Event)</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>review41.txt</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>montón, préstamo, plata</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>plata (Product), 3 semanas (DateTime)</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>review64.txt</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>trámites, gran avance, sucursal</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>sucursal (Location), digital (Skill)</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>review8.txt</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>varios documentos, trámite, proceso, media, personal</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>una semana y media (DateTime), personal (PersonType)</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>review35.txt</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>información contradictoria, atención, sucursal, asesor, pasos, desastre, servicio</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>sucursal (Location), asesor (PersonType)</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles), United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>review45.txt</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>papa caliente, Nadie, sucursal, asesor, desorden</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>sucursal (Location), asesor (PersonType), papa (PersonType), desorden (Event)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>review53.txt</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>banco, era, piedra, mano</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>banco (Location)</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>review74.txt</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Tasa Efectiva Anual, trámites, TEA</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>primera (Quantity), Anual (DateTime)</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Tasa (https://en.wikipedia.org/wiki/Tasa), Tea (https://en.wikipedia.org/wiki/Tea)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>review31.txt</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Demasiada burocracia, proceso, solicitud, laberinto, oficina, papeles, diferentes</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>3 (Quantity), oficina (Location), burocracia (Skill)</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>review5.txt</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>tres días, Caja ADV, experiencia, solicitud, desembolso</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>tres días (DateTime), ADV (Skill)</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Mii (https://en.wikipedia.org/wiki/Mii)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>review15.txt</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>buena tasa de, Buen servicio, interés, WhatsApp, dudas</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>cuatro días (DateTime), WhatsApp (Organization)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>review65.txt</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>préstamo, urgencia, plazos, eficiencia, equipo</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>review79.txt</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>interés, flujo, tasa</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Él (film) (https://en.wikipedia.org/wiki/Él_(film))</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>review21.txt</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>tres días, préstamo, dos semanas, Nadie, respuesta, clara</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>dos semanas (DateTime)</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>review56.txt</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>50 hojas, proceso</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>50 (Quantity), 100% (Quantity)</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>review12.txt</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>diez días, evaluación, atención, comunicación, desembolso, avance</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>diez días (DateTime), comunicación (Skill)</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>review48.txt</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Poca transparencia, seguros, comisiones, cuota</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>seguros (Skill)</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Poca, West Virginia (https://en.wikipedia.org/wiki/Poca,_West_Virginia)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>review28.txt</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>pésima experiencia, Caja ADV, documentos, errores, nada</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>documentos (Product), Caja ADV (Organization)</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Spondias mombin (https://en.wikipedia.org/wiki/Spondias_mombin)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>review27.txt</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>mucha gente, una hora, agencia, sistema</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>agencia (Location), una hora (DateTime), ágil (Skill)</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>English language (https://en.wikipedia.org/wiki/English_language)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>review60.txt</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>obstáculo, formato, documentos</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>review57.txt</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>documentación, manos, error</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>documentación (Skill)</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>.se (https://en.wikipedia.org/wiki/.se)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>review46.txt</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>pura tramitología, aprobación, dinero</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>review43.txt</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>La TEA, pura publicidad, inicio, tasa, infarto</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>TEA (Product), infarto (Event)</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin), Tea (https://en.wikipedia.org/wiki/Tea)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>review71.txt</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>gestión, tasa, papeleo, punto, costo</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>papeleo (Product), gestión (Skill)</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Los Angeles (https://en.wikipedia.org/wiki/Los_Angeles), United Nations (https://en.wikipedia.org/wiki/United_Nations)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>review34.txt</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>misma información, tres formatos distintos, Cero digitalización, trámites</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>digitalización (Skill)</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Computer Entertainment Rating Organization (https://en.wikipedia.org/wiki/Computer_Entertainment_Rating_Organization)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>review62.txt</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>documentación, día, desembolso, dinero, cuenta</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>United Nationalist Alliance (https://en.wikipedia.org/wiki/United_Nationalist_Alliance)</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>review20.txt</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>dos días, préstamo, estudios, asesor, momento, cliente</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>dos días (DateTime), asesor (PersonType), cliente (PersonType)</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>review38.txt</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>TEA, tiempo, papeleo</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>TEA (Organization), papeleo (Skill)</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Sinceramente (https://en.wikipedia.org/wiki/Sinceramente), Tea (https://en.wikipedia.org/wiki/Tea)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>review42.txt</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>papeleo, martirio, copia</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>copia (Product)</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>El (deity) (https://en.wikipedia.org/wiki/El_(deity))</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>review51.txt</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>evaluación crediticia, proceso, sentido, historial</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>proceso (Event), evaluación crediticia (Event), revisar (Skill)</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Tienen (https://en.wikipedia.org/wiki/Tienen)</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>review59.txt</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>experiencia agotadora, nadie</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>United Nationalist Alliance (https://en.wikipedia.org/wiki/United_Nationalist_Alliance)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>review3.txt</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Excelente servicio, préstamo, trámite, negocio, 48 horas, paso</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>servicio (Skill), 48 horas (DateTime)</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Dobla (https://en.wikipedia.org/wiki/Dobla), Ped- (https://en.wikipedia.org/wiki/Ped-)</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>review63.txt</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>pre-aprobación, flujo, solicitud, casa, problemas</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>casa (Location)</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Él (film) (https://en.wikipedia.org/wiki/Él_(film))</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>review50.txt</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Pésimo manejo, otro lado, Tardaron, tiempos</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>manejo (Skill), tiempos (Skill)</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>review11.txt</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>tres días, Caja ADV, préstamo, buena experiencia, agencia, respeto, rapidez</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>agencia (Location), Caja ADV (Organization), tres días (DateTime)</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>English language (https://en.wikipedia.org/wiki/English_language), Isidoro Caja de la Jara (https://en.wikipedia.org/wiki/Isidoro_Caja_de_la_Jara), El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>review44.txt</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>aplicación, trámite, seguimiento, chiste, rato</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>aplicación (Skill), trámite (Event)</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Latin America (https://en.wikipedia.org/wiki/Latin_America)</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>review49.txt</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>letra chica, tasa preferencial, Falsa publicidad, La, monto</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>publicidad (Skill)</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin)</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>review52.txt</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>mixed</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Cero empatía, asesora, cara, Maltrato, cliente</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>asesora (PersonType), Maltrato (Skill), cliente (PersonType)</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin), Computer Entertainment Rating Organization (https://en.wikipedia.org/wiki/Computer_Entertainment_Rating_Organization)</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>review4.txt</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>nueve días, préstamo, proceso, trato, tiempos</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>nueve días (DateTime)</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>El Préstamo (https://en.wikipedia.org/wiki/El_Préstamo)</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>review40.txt</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>cláusulas ocultas, cliente promedio, comisiones, seguros, contrato</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>comisiones (Organization), seguros (Skill), cliente (PersonType)</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Hay (https://en.wikipedia.org/wiki/Hay)</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>review77.txt</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>banco anterior, tasa</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>banco (Location)</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Latin (https://en.wikipedia.org/wiki/Latin)</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>review69.txt</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>préstamo, Me ayudaron, deudas, ahorro, intereses, mensuales, finanzas</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>mensuales (DateTime), finanzas (Skill)</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>review37.txt</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Una decepción total, artículo, lentitud, desembolso, oportunidad, descuento</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>United Nationalist Alliance (https://en.wikipedia.org/wiki/United_Nationalist_Alliance)</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>review76.txt</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>trámites, verdad</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>review9.txt</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Spanish</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
         <is>
           <t>positive</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>dos días, trámite, línea, desembolso, correo, paso, proceso</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>dos días (DateTime), correo (Product)</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>review47.txt</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>vacunación, digitalización, carné, perro, requisitos, pilas</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>pilas (Product), digitalización (Skill)</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>review54.txt</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Super mala onda, último momento, condiciones</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Súper (https://en.wikipedia.org/wiki/Súper)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>